<commit_message>
Added bar codes and recovery dates where necessary CP04OSPM
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP04OSPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CP04OSPM_00001.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="9600" yWindow="9630" windowWidth="20730" windowHeight="9810" tabRatio="377" activeTab="1"/>
   </bookViews>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
   <si>
     <t>Ref Des</t>
   </si>
@@ -220,9 +225,6 @@
     <t>SWE 0004-G</t>
   </si>
   <si>
-    <t>This serial number is a placekeeper used until the correct serial number is found or defined</t>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -254,6 +256,12 @@
   </si>
   <si>
     <t>N00093</t>
+  </si>
+  <si>
+    <t>OL000342</t>
+  </si>
+  <si>
+    <t>OL000252</t>
   </si>
 </sst>
 </file>
@@ -628,7 +636,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -663,7 +671,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -875,7 +883,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -932,7 +940,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>33</v>
@@ -993,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1013,7 @@
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1014,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -1023,7 +1031,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -1050,7 +1058,7 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>40</v>
@@ -1059,10 +1067,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>16</v>
@@ -1077,7 +1085,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>40</v>
@@ -1086,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>14</v>
@@ -1104,7 +1112,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>40</v>
@@ -1113,10 +1121,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>15</v>
@@ -1131,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>40</v>
@@ -1140,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>17</v>
@@ -1158,7 +1166,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>40</v>
@@ -1167,10 +1175,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1185,7 +1193,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>40</v>
@@ -1194,10 +1202,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>19</v>
@@ -1212,7 +1220,7 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>40</v>
@@ -1221,10 +1229,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>20</v>
@@ -1239,7 +1247,7 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>40</v>
@@ -1248,10 +1256,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>21</v>
@@ -1277,7 +1285,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>40</v>
@@ -1286,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="11">
         <v>126</v>
@@ -1304,7 +1312,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>40</v>
@@ -1313,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="11">
         <v>126</v>
@@ -1342,7 +1350,7 @@
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>40</v>
@@ -1351,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="12">
         <v>100036</v>
@@ -1369,7 +1377,7 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>40</v>
@@ -1378,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16" s="12">
         <v>100036</v>
@@ -1407,7 +1415,7 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>40</v>
@@ -1416,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="15">
         <v>1118</v>
@@ -1434,7 +1442,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>40</v>
@@ -1443,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="11">
         <v>1118</v>
@@ -1461,7 +1469,7 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>40</v>
@@ -1470,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="11">
         <v>1118</v>
@@ -1488,7 +1496,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>40</v>
@@ -1497,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="11">
         <v>1118</v>
@@ -1515,7 +1523,7 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>40</v>
@@ -1524,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="11">
         <v>1118</v>
@@ -1542,7 +1550,7 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>40</v>
@@ -1551,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="11">
         <v>1118</v>
@@ -1569,7 +1577,7 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>40</v>
@@ -1578,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" s="11">
         <v>1118</v>
@@ -1596,7 +1604,7 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>40</v>
@@ -1605,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" s="11">
         <v>1118</v>
@@ -1623,7 +1631,7 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>40</v>
@@ -1632,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" s="11">
         <v>1118</v>
@@ -1650,7 +1658,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>40</v>
@@ -1659,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="11">
         <v>1118</v>
@@ -1688,7 +1696,7 @@
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>40</v>
@@ -1697,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" s="11">
         <v>20468</v>
@@ -1715,7 +1723,7 @@
         <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>40</v>
@@ -1724,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" s="11">
         <v>20468</v>
@@ -1753,7 +1761,7 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>40</v>
@@ -1762,10 +1770,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -1787,7 +1795,7 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>40</v>
@@ -1795,14 +1803,14 @@
       <c r="D34" s="11">
         <v>1</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
       <c r="F34" s="25" t="s">
         <v>51</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="H34" s="10"/>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1821,7 +1829,7 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>40</v>
@@ -1829,7 +1837,9 @@
       <c r="D36" s="11">
         <v>1</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
       <c r="F36" s="11" t="s">
         <v>41</v>
       </c>

</xml_diff>